<commit_message>
muir_l.py has been added for decade inductors. This imports calculate_imp.py and uses selected methods appropriate to the inductors.
</commit_message>
<xml_diff>
--- a/coaxCap_Results.xlsx
+++ b/coaxCap_Results.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="pyUBresults" sheetId="1" state="visible" r:id="rId1"/>
@@ -44,15 +44,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -436,16 +436,16 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E2" t="n">
-        <v>-4</v>
+        <v>10</v>
       </c>
       <c r="F2" t="n">
-        <v>1591.5</v>
+        <v>1594.12</v>
       </c>
       <c r="G2" t="n">
-        <v>19.63</v>
+        <v>19.65</v>
       </c>
       <c r="H2" t="n">
         <v>0.2</v>
@@ -457,7 +457,7 @@
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>0.0001</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
         <v>10</v>
@@ -466,7 +466,7 @@
         <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>6.999999999999999e-05</v>
+        <v>0</v>
       </c>
       <c r="O2" t="n">
         <v>10</v>
@@ -499,10 +499,10 @@
         <v>0</v>
       </c>
       <c r="Y2" t="n">
-        <v>1.256676091737355e-16</v>
+        <v>1.034588057504798e-16</v>
       </c>
       <c r="Z2" t="n">
-        <v>0</v>
+        <v>2.433896954542872e-12</v>
       </c>
     </row>
     <row r="3">
@@ -520,16 +520,16 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>999801</v>
+        <v>999817</v>
       </c>
       <c r="E3" t="n">
-        <v>1696</v>
+        <v>1640</v>
       </c>
       <c r="F3" t="n">
-        <v>1591.5</v>
+        <v>1593.2</v>
       </c>
       <c r="G3" t="n">
-        <v>19.63</v>
+        <v>20.04</v>
       </c>
       <c r="H3" t="n">
         <v>0.2</v>
@@ -541,7 +541,7 @@
         <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>0.0001</v>
+        <v>2.75e-05</v>
       </c>
       <c r="L3" t="n">
         <v>10</v>
@@ -550,43 +550,43 @@
         <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>6.999999999999999e-05</v>
+        <v>0</v>
       </c>
       <c r="O3" t="n">
         <v>10</v>
       </c>
       <c r="P3" t="n">
-        <v>9.999038740547188e-07</v>
+        <v>9.999208758039257e-07</v>
       </c>
       <c r="Q3" t="n">
-        <v>1.405303984356189e-10</v>
+        <v>4.516455053091704e-11</v>
       </c>
       <c r="R3" t="n">
-        <v>2.076018652788616</v>
+        <v>2.023240151271259</v>
       </c>
       <c r="S3" t="n">
-        <v>1.699934213652265e-06</v>
+        <v>1.629936922501878e-06</v>
       </c>
       <c r="T3" t="n">
-        <v>3.781878929066422e-07</v>
+        <v>3.789946124422143e-07</v>
       </c>
       <c r="U3" t="n">
-        <v>2.218363017792686</v>
+        <v>2.218414459480953</v>
       </c>
       <c r="V3" t="n">
-        <v>0.170015042465217</v>
+        <v>0.1630116514466714</v>
       </c>
       <c r="W3" t="n">
-        <v>0.03782360157281184</v>
+        <v>0.03790363750743998</v>
       </c>
       <c r="X3" t="n">
-        <v>2.218362900451228</v>
+        <v>2.2184144569907</v>
       </c>
       <c r="Y3" t="n">
-        <v>2.199801089681299e-11</v>
+        <v>2.199836279894013e-11</v>
       </c>
       <c r="Z3" t="n">
-        <v>2.699683609591658e-07</v>
+        <v>2.702610592513617e-07</v>
       </c>
     </row>
     <row r="4">
@@ -604,16 +604,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E4" t="n">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>1591.5</v>
+        <v>1592.78</v>
       </c>
       <c r="G4" t="n">
-        <v>19.66</v>
+        <v>20.08</v>
       </c>
       <c r="H4" t="n">
         <v>0.2</v>
@@ -625,7 +625,7 @@
         <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>0.0001</v>
+        <v>0</v>
       </c>
       <c r="L4" t="n">
         <v>10</v>
@@ -634,7 +634,7 @@
         <v>0</v>
       </c>
       <c r="N4" t="n">
-        <v>6.999999999999999e-05</v>
+        <v>0</v>
       </c>
       <c r="O4" t="n">
         <v>10</v>
@@ -667,10 +667,10 @@
         <v>0</v>
       </c>
       <c r="Y4" t="n">
-        <v>1.256676091737355e-16</v>
+        <v>1.233663930019391e-16</v>
       </c>
       <c r="Z4" t="n">
-        <v>0</v>
+        <v>2.67506395485076e-12</v>
       </c>
     </row>
     <row r="5">
@@ -688,16 +688,16 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>999928</v>
+        <v>999944</v>
       </c>
       <c r="E5" t="n">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="F5" t="n">
-        <v>1591.5</v>
+        <v>1591.89</v>
       </c>
       <c r="G5" t="n">
-        <v>19.66</v>
+        <v>20.11</v>
       </c>
       <c r="H5" t="n">
         <v>0.2</v>
@@ -709,7 +709,7 @@
         <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>0.0001</v>
+        <v>2.75e-05</v>
       </c>
       <c r="L5" t="n">
         <v>10</v>
@@ -718,43 +718,43 @@
         <v>0</v>
       </c>
       <c r="N5" t="n">
-        <v>6.999999999999999e-05</v>
+        <v>0</v>
       </c>
       <c r="O5" t="n">
         <v>10</v>
       </c>
       <c r="P5" t="n">
-        <v>1.000030887122324e-07</v>
+        <v>1.000047888871531e-07</v>
       </c>
       <c r="Q5" t="n">
-        <v>1.369931424950706e-11</v>
+        <v>4.552348543349149e-12</v>
       </c>
       <c r="R5" t="n">
-        <v>2.072233187172548</v>
+        <v>2.023004113939691</v>
       </c>
       <c r="S5" t="n">
-        <v>3.969846369529113e-08</v>
+        <v>3.959846756507628e-08</v>
       </c>
       <c r="T5" t="n">
-        <v>3.782355342204783e-08</v>
+        <v>3.784252074943758e-08</v>
       </c>
       <c r="U5" t="n">
-        <v>2.218365552954695</v>
+        <v>2.218379278774329</v>
       </c>
       <c r="V5" t="n">
-        <v>0.03969847051048737</v>
+        <v>0.03959780115212037</v>
       </c>
       <c r="W5" t="n">
-        <v>0.0378235600249397</v>
+        <v>0.0378418839101956</v>
       </c>
       <c r="X5" t="n">
-        <v>2.218365547192596</v>
+        <v>2.218379278602178</v>
       </c>
       <c r="Y5" t="n">
-        <v>2.200193619278286e-12</v>
+        <v>2.200228792112639e-12</v>
       </c>
       <c r="Z5" t="n">
-        <v>2.700269526676002e-08</v>
+        <v>2.700974446376493e-08</v>
       </c>
     </row>
     <row r="6">
@@ -775,13 +775,13 @@
         <v>-1</v>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F6" t="n">
-        <v>1591.5</v>
+        <v>1592.17</v>
       </c>
       <c r="G6" t="n">
-        <v>19.63</v>
+        <v>20.47</v>
       </c>
       <c r="H6" t="n">
         <v>0.2</v>
@@ -793,7 +793,7 @@
         <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>0.0001</v>
+        <v>0</v>
       </c>
       <c r="L6" t="n">
         <v>10</v>
@@ -802,7 +802,7 @@
         <v>0</v>
       </c>
       <c r="N6" t="n">
-        <v>6.999999999999999e-05</v>
+        <v>0</v>
       </c>
       <c r="O6" t="n">
         <v>10</v>
@@ -835,10 +835,10 @@
         <v>0</v>
       </c>
       <c r="Y6" t="n">
-        <v>1.254475865369387e-16</v>
+        <v>1.25394704433805e-16</v>
       </c>
       <c r="Z6" t="n">
-        <v>2.697215948472578e-12</v>
+        <v>2.698351439949472e-12</v>
       </c>
     </row>
     <row r="7">
@@ -856,16 +856,16 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>999986</v>
+        <v>1000003</v>
       </c>
       <c r="E7" t="n">
-        <v>496</v>
+        <v>479</v>
       </c>
       <c r="F7" t="n">
-        <v>1591.5</v>
+        <v>1592.19</v>
       </c>
       <c r="G7" t="n">
-        <v>19.64</v>
+        <v>20.21</v>
       </c>
       <c r="H7" t="n">
         <v>0.2</v>
@@ -877,7 +877,7 @@
         <v>0</v>
       </c>
       <c r="K7" t="n">
-        <v>0.0001</v>
+        <v>2.75e-05</v>
       </c>
       <c r="L7" t="n">
         <v>10</v>
@@ -886,43 +886,43 @@
         <v>0</v>
       </c>
       <c r="N7" t="n">
-        <v>6.999999999999999e-05</v>
+        <v>0</v>
       </c>
       <c r="O7" t="n">
         <v>10</v>
       </c>
       <c r="P7" t="n">
-        <v>1.000089893193101e-08</v>
+        <v>1.000106894942308e-08</v>
       </c>
       <c r="Q7" t="n">
-        <v>1.393457953591975e-12</v>
+        <v>4.659875191787677e-13</v>
       </c>
       <c r="R7" t="n">
-        <v>2.074727724798973</v>
+        <v>2.022888385509832</v>
       </c>
       <c r="S7" t="n">
-        <v>4.929809219591567e-09</v>
+        <v>4.749816185204857e-09</v>
       </c>
       <c r="T7" t="n">
-        <v>3.782576767468423e-09</v>
+        <v>3.785890133436816e-09</v>
       </c>
       <c r="U7" t="n">
-        <v>2.218366666615906</v>
+        <v>2.218386761343267</v>
       </c>
       <c r="V7" t="n">
-        <v>0.04929519201933456</v>
+        <v>0.04749456014900783</v>
       </c>
       <c r="W7" t="n">
-        <v>0.03782354258531394</v>
+        <v>0.03785603059362858</v>
       </c>
       <c r="X7" t="n">
-        <v>2.218366657189203</v>
+        <v>2.218386760987068</v>
       </c>
       <c r="Y7" t="n">
-        <v>2.201452240890192e-13</v>
+        <v>2.201489100138555e-13</v>
       </c>
       <c r="Z7" t="n">
-        <v>2.702856062453225e-09</v>
+        <v>2.704073817686499e-09</v>
       </c>
     </row>
     <row r="8">
@@ -943,13 +943,13 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="F8" t="n">
-        <v>1591.5</v>
+        <v>1592.13</v>
       </c>
       <c r="G8" t="n">
-        <v>19.65</v>
+        <v>20.61</v>
       </c>
       <c r="H8" t="n">
         <v>0.2</v>
@@ -961,7 +961,7 @@
         <v>0</v>
       </c>
       <c r="K8" t="n">
-        <v>0.0001</v>
+        <v>0</v>
       </c>
       <c r="L8" t="n">
         <v>10</v>
@@ -970,7 +970,7 @@
         <v>0</v>
       </c>
       <c r="N8" t="n">
-        <v>6.999999999999999e-05</v>
+        <v>0</v>
       </c>
       <c r="O8" t="n">
         <v>10</v>
@@ -1003,7 +1003,7 @@
         <v>0</v>
       </c>
       <c r="Y8" t="n">
-        <v>1.256676091737355e-16</v>
+        <v>1.256178829618184e-16</v>
       </c>
       <c r="Z8" t="n">
         <v>0</v>
@@ -1024,16 +1024,16 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>999660</v>
+        <v>999707</v>
       </c>
       <c r="E9" t="n">
-        <v>-205</v>
+        <v>-218</v>
       </c>
       <c r="F9" t="n">
-        <v>1591.5</v>
+        <v>1592.07</v>
       </c>
       <c r="G9" t="n">
-        <v>19.64</v>
+        <v>20.19</v>
       </c>
       <c r="H9" t="n">
         <v>0.2</v>
@@ -1045,7 +1045,7 @@
         <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>0.0001</v>
+        <v>9e-06</v>
       </c>
       <c r="L9" t="n">
         <v>10</v>
@@ -1054,43 +1054,43 @@
         <v>0</v>
       </c>
       <c r="N9" t="n">
-        <v>6.999999999999999e-05</v>
+        <v>0</v>
       </c>
       <c r="O9" t="n">
         <v>10</v>
       </c>
       <c r="P9" t="n">
-        <v>9.998258450917296e-10</v>
+        <v>9.998728528891004e-10</v>
       </c>
       <c r="Q9" t="n">
-        <v>1.393091742146596e-13</v>
+        <v>3.565722513400956e-14</v>
       </c>
       <c r="R9" t="n">
-        <v>2.074727582702421</v>
+        <v>2.076177969564305</v>
       </c>
       <c r="S9" t="n">
-        <v>-2.280055404445766e-10</v>
+        <v>-2.300055890449676e-10</v>
       </c>
       <c r="T9" t="n">
-        <v>3.78158779752721e-10</v>
+        <v>3.784447589842954e-10</v>
       </c>
       <c r="U9" t="n">
-        <v>2.21836047700562</v>
+        <v>2.21837789659931</v>
       </c>
       <c r="V9" t="n">
-        <v>-0.02280523385377906</v>
+        <v>-0.02300419819965971</v>
       </c>
       <c r="W9" t="n">
-        <v>0.03782363971846654</v>
+        <v>0.03785046389708496</v>
       </c>
       <c r="X9" t="n">
-        <v>2.218360474759064</v>
+        <v>2.218377896754195</v>
       </c>
       <c r="Y9" t="n">
-        <v>2.212183620119179e-14</v>
+        <v>2.212282538065619e-14</v>
       </c>
       <c r="Z9" t="n">
-        <v>2.726445100197699e-10</v>
+        <v>2.727548546400607e-10</v>
       </c>
     </row>
     <row r="10">
@@ -1108,16 +1108,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>999863</v>
+        <v>999876</v>
       </c>
       <c r="E10" t="n">
-        <v>-136</v>
+        <v>-158</v>
       </c>
       <c r="F10" t="n">
-        <v>1591.5</v>
+        <v>1591.9</v>
       </c>
       <c r="G10" t="n">
-        <v>19.64</v>
+        <v>20.8</v>
       </c>
       <c r="H10" t="n">
         <v>0.2</v>
@@ -1129,7 +1129,7 @@
         <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>0.0001</v>
+        <v>1e-06</v>
       </c>
       <c r="L10" t="n">
         <v>10</v>
@@ -1138,43 +1138,43 @@
         <v>0</v>
       </c>
       <c r="N10" t="n">
-        <v>6.999999999999999e-05</v>
+        <v>0</v>
       </c>
       <c r="O10" t="n">
         <v>10</v>
       </c>
       <c r="P10" t="n">
-        <v>1.000028878769734e-09</v>
+        <v>1.000041880926454e-09</v>
       </c>
       <c r="Q10" t="n">
-        <v>1.393374406392102e-13</v>
+        <v>3.428163893434152e-14</v>
       </c>
       <c r="R10" t="n">
-        <v>2.074727686837524</v>
+        <v>2.10362861939283</v>
       </c>
       <c r="S10" t="n">
-        <v>-1.590038637310863e-10</v>
+        <v>-1.700041310332369e-10</v>
       </c>
       <c r="T10" t="n">
-        <v>3.782349672142469e-10</v>
+        <v>3.784281038733997e-10</v>
       </c>
       <c r="U10" t="n">
-        <v>2.218364327076741</v>
+        <v>2.218376634738403</v>
       </c>
       <c r="V10" t="n">
-        <v>-0.01590042104247075</v>
+        <v>-0.01700022913772975</v>
       </c>
       <c r="W10" t="n">
-        <v>0.03782357921305569</v>
+        <v>0.03784240088320211</v>
       </c>
       <c r="X10" t="n">
-        <v>2.218364325939026</v>
+        <v>2.218376634837701</v>
       </c>
       <c r="Y10" t="n">
-        <v>2.212630294210788e-14</v>
+        <v>2.212655741279608e-14</v>
       </c>
       <c r="Z10" t="n">
-        <v>2.726993274102398e-10</v>
+        <v>2.727713777108246e-10</v>
       </c>
     </row>
     <row r="11">
@@ -1192,16 +1192,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>999878</v>
+        <v>999859</v>
       </c>
       <c r="E11" t="n">
-        <v>-170</v>
+        <v>-138</v>
       </c>
       <c r="F11" t="n">
-        <v>1591.5</v>
+        <v>1591.86</v>
       </c>
       <c r="G11" t="n">
-        <v>19.64</v>
+        <v>20.8</v>
       </c>
       <c r="H11" t="n">
         <v>0.2</v>
@@ -1213,7 +1213,7 @@
         <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>0.0001</v>
+        <v>1e-06</v>
       </c>
       <c r="L11" t="n">
         <v>10</v>
@@ -1222,43 +1222,43 @@
         <v>0</v>
       </c>
       <c r="N11" t="n">
-        <v>6.999999999999999e-05</v>
+        <v>0</v>
       </c>
       <c r="O11" t="n">
         <v>10</v>
       </c>
       <c r="P11" t="n">
-        <v>1.000043881258257e-09</v>
+        <v>1.000024878106128e-09</v>
       </c>
       <c r="Q11" t="n">
-        <v>1.393395292919275e-13</v>
+        <v>3.428106579316784e-14</v>
       </c>
       <c r="R11" t="n">
-        <v>2.074727694527584</v>
+        <v>2.103628376104718</v>
       </c>
       <c r="S11" t="n">
-        <v>-1.930046899377337e-10</v>
+        <v>-1.500036450293267e-10</v>
       </c>
       <c r="T11" t="n">
-        <v>3.782405969233787e-10</v>
+        <v>3.784028682873857e-10</v>
       </c>
       <c r="U11" t="n">
-        <v>2.218364610906618</v>
+        <v>2.21837526293537</v>
       </c>
       <c r="V11" t="n">
-        <v>-0.01930022153294946</v>
+        <v>-0.01500045722006737</v>
       </c>
       <c r="W11" t="n">
-        <v>0.0378235747616124</v>
+        <v>0.03784052072088269</v>
       </c>
       <c r="X11" t="n">
-        <v>2.21836460926945</v>
+        <v>2.218375263012689</v>
       </c>
       <c r="Y11" t="n">
-        <v>2.212663299685539e-14</v>
+        <v>2.212618650771077e-14</v>
       </c>
       <c r="Z11" t="n">
-        <v>2.727033779563337e-10</v>
+        <v>2.727599320707821e-10</v>
       </c>
     </row>
     <row r="12">
@@ -1276,16 +1276,16 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E12" t="n">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="F12" t="n">
-        <v>1591.5</v>
+        <v>1595.3</v>
       </c>
       <c r="G12" t="n">
-        <v>19.63</v>
+        <v>19.9</v>
       </c>
       <c r="H12" t="n">
         <v>0.2</v>
@@ -1297,7 +1297,7 @@
         <v>0</v>
       </c>
       <c r="K12" t="n">
-        <v>0.0001</v>
+        <v>0</v>
       </c>
       <c r="L12" t="n">
         <v>10</v>
@@ -1306,7 +1306,7 @@
         <v>0</v>
       </c>
       <c r="N12" t="n">
-        <v>6.999999999999999e-05</v>
+        <v>0</v>
       </c>
       <c r="O12" t="n">
         <v>10</v>
@@ -1339,10 +1339,10 @@
         <v>0</v>
       </c>
       <c r="Y12" t="n">
-        <v>1.256808103801378e-16</v>
+        <v>1.253792702963777e-16</v>
       </c>
       <c r="Z12" t="n">
-        <v>2.700078152195537e-12</v>
+        <v>2.706498021048579e-12</v>
       </c>
     </row>
     <row r="13">
@@ -1360,16 +1360,16 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>999865</v>
+        <v>999917</v>
       </c>
       <c r="E13" t="n">
-        <v>2540</v>
+        <v>2270</v>
       </c>
       <c r="F13" t="n">
-        <v>1591.5</v>
+        <v>1595.12</v>
       </c>
       <c r="G13" t="n">
-        <v>19.64</v>
+        <v>20.02</v>
       </c>
       <c r="H13" t="n">
         <v>0.2</v>
@@ -1381,7 +1381,7 @@
         <v>0</v>
       </c>
       <c r="K13" t="n">
-        <v>0.0001</v>
+        <v>9e-06</v>
       </c>
       <c r="L13" t="n">
         <v>10</v>
@@ -1390,43 +1390,43 @@
         <v>0</v>
       </c>
       <c r="N13" t="n">
-        <v>6.999999999999999e-05</v>
+        <v>0</v>
       </c>
       <c r="O13" t="n">
         <v>10</v>
       </c>
       <c r="P13" t="n">
-        <v>9.999503812291006e-11</v>
+        <v>1.000003386072989e-10</v>
       </c>
       <c r="Q13" t="n">
-        <v>1.393272970057299e-14</v>
+        <v>3.55239852036184e-15</v>
       </c>
       <c r="R13" t="n">
-        <v>2.074727849473021</v>
+        <v>2.078393745352665</v>
       </c>
       <c r="S13" t="n">
-        <v>2.525873203291238e-10</v>
+        <v>2.239887559529839e-10</v>
       </c>
       <c r="T13" t="n">
-        <v>3.782053356198552e-11</v>
+        <v>3.799313632024773e-11</v>
       </c>
       <c r="U13" t="n">
-        <v>2.218363954780115</v>
+        <v>2.218469092673973</v>
       </c>
       <c r="V13" t="n">
-        <v>0.252607694231861</v>
+        <v>0.2239949506835178</v>
       </c>
       <c r="W13" t="n">
-        <v>0.03782358885789559</v>
+        <v>0.03799418746939371</v>
       </c>
       <c r="X13" t="n">
-        <v>2.218363707097192</v>
+        <v>2.218469107537312</v>
       </c>
       <c r="Y13" t="n">
-        <v>2.325571649084159e-15</v>
+        <v>2.325400866735839e-15</v>
       </c>
       <c r="Z13" t="n">
-        <v>2.969789991120639e-11</v>
+        <v>2.976685754945776e-11</v>
       </c>
     </row>
     <row r="14">
@@ -1444,16 +1444,16 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>99969</v>
+        <v>99984</v>
       </c>
       <c r="E14" t="n">
-        <v>260</v>
+        <v>240</v>
       </c>
       <c r="F14" t="n">
-        <v>1591.5</v>
+        <v>1592.93</v>
       </c>
       <c r="G14" t="n">
-        <v>19.64</v>
+        <v>20</v>
       </c>
       <c r="H14" t="n">
         <v>0.2</v>
@@ -1465,7 +1465,7 @@
         <v>0</v>
       </c>
       <c r="K14" t="n">
-        <v>0.0001</v>
+        <v>9e-06</v>
       </c>
       <c r="L14" t="n">
         <v>10</v>
@@ -1474,43 +1474,43 @@
         <v>0</v>
       </c>
       <c r="N14" t="n">
-        <v>6.999999999999999e-05</v>
+        <v>0</v>
       </c>
       <c r="O14" t="n">
         <v>10</v>
       </c>
       <c r="P14" t="n">
-        <v>9.997213602998481e-12</v>
+        <v>9.998813749229067e-12</v>
       </c>
       <c r="Q14" t="n">
-        <v>1.449335960139864e-15</v>
+        <v>5.530009498881907e-16</v>
       </c>
       <c r="R14" t="n">
-        <v>2.053653812520978</v>
+        <v>2.000815441738256</v>
       </c>
       <c r="S14" t="n">
-        <v>2.459876516269377e-11</v>
+        <v>2.099894587059224e-11</v>
       </c>
       <c r="T14" t="n">
-        <v>5.575855710561372e-12</v>
+        <v>5.577920745996919e-12</v>
       </c>
       <c r="U14" t="n">
-        <v>2.018723944582334</v>
+        <v>2.018848486255812</v>
       </c>
       <c r="V14" t="n">
-        <v>0.24606385003045</v>
+        <v>0.2100208914940808</v>
       </c>
       <c r="W14" t="n">
-        <v>0.05577583278393387</v>
+        <v>0.05578755672234557</v>
       </c>
       <c r="X14" t="n">
-        <v>2.018723925355017</v>
+        <v>2.01884848617405</v>
       </c>
       <c r="Y14" t="n">
-        <v>3.456195096461043e-16</v>
+        <v>3.455396987398924e-16</v>
       </c>
       <c r="Z14" t="n">
-        <v>5.399241990792781e-12</v>
+        <v>5.404498724452729e-12</v>
       </c>
     </row>
     <row r="15">
@@ -1528,16 +1528,16 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>10004</v>
+        <v>10003</v>
       </c>
       <c r="E15" t="n">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="F15" t="n">
-        <v>1591.5</v>
+        <v>1594.62</v>
       </c>
       <c r="G15" t="n">
-        <v>19.61</v>
+        <v>19.96</v>
       </c>
       <c r="H15" t="n">
         <v>0.2</v>
@@ -1549,7 +1549,7 @@
         <v>0</v>
       </c>
       <c r="K15" t="n">
-        <v>0.0001</v>
+        <v>1.2e-05</v>
       </c>
       <c r="L15" t="n">
         <v>10</v>
@@ -1558,7 +1558,7 @@
         <v>0</v>
       </c>
       <c r="N15" t="n">
-        <v>6.999999999999999e-05</v>
+        <v>0</v>
       </c>
       <c r="O15" t="n">
         <v>10</v>
@@ -1567,34 +1567,34 @@
         <v>9.99891375836848e-13</v>
       </c>
       <c r="Q15" t="n">
-        <v>4.609779958709705e-16</v>
+        <v>4.427353131389402e-16</v>
       </c>
       <c r="R15" t="n">
-        <v>2.012593994184846</v>
+        <v>2.021871798193535</v>
       </c>
       <c r="S15" t="n">
-        <v>2.599869488739992e-12</v>
+        <v>1.999899606723071e-12</v>
       </c>
       <c r="T15" t="n">
-        <v>4.429906379852272e-12</v>
+        <v>4.425964763871571e-12</v>
       </c>
       <c r="U15" t="n">
-        <v>2.021964842564447</v>
+        <v>2.021927365067199</v>
       </c>
       <c r="V15" t="n">
-        <v>0.2600232628433888</v>
+        <v>0.2000178963354084</v>
       </c>
       <c r="W15" t="n">
-        <v>0.4430525066899784</v>
+        <v>0.4426582965782722</v>
       </c>
       <c r="X15" t="n">
-        <v>2.021964833678469</v>
+        <v>2.02192735994078</v>
       </c>
       <c r="Y15" t="n">
-        <v>1.476784206485485e-16</v>
+        <v>1.474303418427843e-16</v>
       </c>
       <c r="Z15" t="n">
-        <v>2.970040438824542e-12</v>
+        <v>2.975835895206265e-12</v>
       </c>
     </row>
     <row r="16">
@@ -1612,16 +1612,16 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>99989</v>
+        <v>99992</v>
       </c>
       <c r="E16" t="n">
-        <v>270</v>
+        <v>225</v>
       </c>
       <c r="F16" t="n">
-        <v>1591.5</v>
+        <v>1594.5</v>
       </c>
       <c r="G16" t="n">
-        <v>19.58</v>
+        <v>20.6</v>
       </c>
       <c r="H16" t="n">
         <v>0.2</v>
@@ -1633,7 +1633,7 @@
         <v>0</v>
       </c>
       <c r="K16" t="n">
-        <v>0.0001</v>
+        <v>1e-06</v>
       </c>
       <c r="L16" t="n">
         <v>10</v>
@@ -1642,43 +1642,43 @@
         <v>0</v>
       </c>
       <c r="N16" t="n">
-        <v>6.999999999999999e-05</v>
+        <v>0</v>
       </c>
       <c r="O16" t="n">
         <v>10</v>
       </c>
       <c r="P16" t="n">
-        <v>9.999213785786712e-12</v>
+        <v>9.999613822344359e-12</v>
       </c>
       <c r="Q16" t="n">
-        <v>1.522283833744776e-15</v>
+        <v>5.439387857512342e-16</v>
       </c>
       <c r="R16" t="n">
-        <v>2.061964313755769</v>
+        <v>2.003742609396941</v>
       </c>
       <c r="S16" t="n">
-        <v>2.55987149660553e-11</v>
+        <v>1.949902116554994e-11</v>
       </c>
       <c r="T16" t="n">
-        <v>5.576301562873049e-12</v>
+        <v>5.581826060699703e-12</v>
       </c>
       <c r="U16" t="n">
-        <v>2.018734029131709</v>
+        <v>2.01896089660569</v>
       </c>
       <c r="V16" t="n">
-        <v>0.2560152231369089</v>
+        <v>0.1950037960594554</v>
       </c>
       <c r="W16" t="n">
-        <v>0.05576913593621972</v>
+        <v>0.05582214911600104</v>
       </c>
       <c r="X16" t="n">
-        <v>2.018734003401803</v>
+        <v>2.018960896683757</v>
       </c>
       <c r="Y16" t="n">
-        <v>3.456635136674454e-16</v>
+        <v>3.454336747425682e-16</v>
       </c>
       <c r="Z16" t="n">
-        <v>5.399782023372555e-12</v>
+        <v>5.410041846408926e-12</v>
       </c>
     </row>
     <row r="17">
@@ -1696,16 +1696,16 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>999840</v>
+        <v>999873</v>
       </c>
       <c r="E17" t="n">
-        <v>2540</v>
+        <v>2265</v>
       </c>
       <c r="F17" t="n">
-        <v>1591.5</v>
+        <v>1593.06</v>
       </c>
       <c r="G17" t="n">
-        <v>19.6</v>
+        <v>20.8</v>
       </c>
       <c r="H17" t="n">
         <v>0.2</v>
@@ -1717,7 +1717,7 @@
         <v>0</v>
       </c>
       <c r="K17" t="n">
-        <v>0.0001</v>
+        <v>1e-06</v>
       </c>
       <c r="L17" t="n">
         <v>10</v>
@@ -1726,46 +1726,46 @@
         <v>0</v>
       </c>
       <c r="N17" t="n">
-        <v>6.999999999999999e-05</v>
+        <v>0</v>
       </c>
       <c r="O17" t="n">
         <v>10</v>
       </c>
       <c r="P17" t="n">
-        <v>9.999253789442474e-11</v>
+        <v>9.999593820516475e-11</v>
       </c>
       <c r="Q17" t="n">
-        <v>1.443116705151015e-14</v>
+        <v>3.427856746129195e-15</v>
       </c>
       <c r="R17" t="n">
-        <v>2.080045418309035</v>
+        <v>2.103634705781022</v>
       </c>
       <c r="S17" t="n">
-        <v>2.525873203291238e-10</v>
+        <v>2.234887810513032e-10</v>
       </c>
       <c r="T17" t="n">
-        <v>3.781959565838107e-11</v>
+        <v>3.789425685746423e-11</v>
       </c>
       <c r="U17" t="n">
-        <v>2.218363461702219</v>
+        <v>2.218414622504492</v>
       </c>
       <c r="V17" t="n">
-        <v>0.2526140104724441</v>
+        <v>0.2235047970472111</v>
       </c>
       <c r="W17" t="n">
-        <v>0.03782359720432302</v>
+        <v>0.03789697285417683</v>
       </c>
       <c r="X17" t="n">
-        <v>2.218363175317335</v>
+        <v>2.218414639620134</v>
       </c>
       <c r="Y17" t="n">
-        <v>2.325516644057482e-15</v>
+        <v>2.325466191002344e-15</v>
       </c>
       <c r="Z17" t="n">
-        <v>2.969722487048167e-11</v>
+        <v>2.972722623579457e-11</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>